<commit_message>
added speedups and compared usb to power supply
</commit_message>
<xml_diff>
--- a/Prac2/Results.xlsx
+++ b/Prac2/Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwolf\Documents\Work\EEE3095S\Prac2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwolf\Documents\Work\eee3095S\Prac2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27B32ACA-C227-466F-AA5D-F6444211A0A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2220979-4A87-4128-8A5E-27E53F7FA9E4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="11355" xr2:uid="{97FB59FB-642C-4C53-A33E-00E9645D38A2}"/>
+    <workbookView xWindow="8280" yWindow="600" windowWidth="21600" windowHeight="13965" xr2:uid="{97FB59FB-642C-4C53-A33E-00E9645D38A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Python</t>
   </si>
@@ -54,12 +54,6 @@
     <t>Threads</t>
   </si>
   <si>
-    <t>ms</t>
-  </si>
-  <si>
-    <t>0.001</t>
-  </si>
-  <si>
     <t>Cflags</t>
   </si>
   <si>
@@ -136,6 +130,30 @@
   </si>
   <si>
     <t>Max speedup</t>
+  </si>
+  <si>
+    <t>On USB</t>
+  </si>
+  <si>
+    <t>On AC Adaptor</t>
+  </si>
+  <si>
+    <t>-Ofast and 32 threads C code</t>
+  </si>
+  <si>
+    <t>Speedup</t>
+  </si>
+  <si>
+    <t>~1A</t>
+  </si>
+  <si>
+    <t>Current delievered</t>
+  </si>
+  <si>
+    <t>Power delivery</t>
+  </si>
+  <si>
+    <t>3A</t>
   </si>
 </sst>
 </file>
@@ -502,24 +520,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37CE9128-54D3-432E-A65E-EEEECA61EB6B}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="I30" sqref="I30:I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>6</v>
       </c>
@@ -536,10 +554,10 @@
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -562,11 +580,14 @@
         <f>AVERAGE(D2:F2)</f>
         <v>6.0050683333333339</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -589,8 +610,20 @@
         <f>AVERAGE(D3:F3)</f>
         <v>3.3383169999999999E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <f>$G$2/G3</f>
+        <v>1798.8310676707258</v>
+      </c>
+      <c r="L3">
+        <f>MIN(G2:G27)</f>
+        <v>1.083161E-3</v>
+      </c>
+      <c r="M3">
+        <f>G2/L3</f>
+        <v>5544.0219259494515</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -610,14 +643,12 @@
         <f t="shared" ref="G4:G27" si="0">AVERAGE(D4:F4)</f>
         <v>5.374456666666666E-3</v>
       </c>
-      <c r="I4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <f t="shared" ref="I4:I26" si="1">$G$2/G4</f>
+        <v>1117.3349616116236</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>2</v>
       </c>
@@ -635,15 +666,11 @@
         <v>2.6631833333333331E-3</v>
       </c>
       <c r="I5">
-        <f>MIN(G2:G27)</f>
-        <v>1.083161E-3</v>
-      </c>
-      <c r="J5">
-        <f>G2/I5</f>
-        <v>5544.0219259494515</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>2254.8460176105041</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>4</v>
       </c>
@@ -660,8 +687,12 @@
         <f t="shared" si="0"/>
         <v>2.5645099999999999E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>2341.6045690339806</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>8</v>
       </c>
@@ -678,8 +709,12 @@
         <f t="shared" si="0"/>
         <v>3.6383666666666668E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>1650.4846497054541</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>16</v>
       </c>
@@ -696,8 +731,12 @@
         <f t="shared" si="0"/>
         <v>2.6182166666666663E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>2293.5719605583959</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>32</v>
       </c>
@@ -714,13 +753,21 @@
         <f t="shared" si="0"/>
         <v>1.9145000000000002E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>3136.6248802994692</v>
+      </c>
+      <c r="L9">
+        <f>6.005068333/0.001083161</f>
+        <v>5544.0219256417095</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D10">
         <v>2.0741599999999998E-3</v>
@@ -735,10 +782,14 @@
         <f t="shared" si="0"/>
         <v>1.9631499999999999E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>3058.8942940342481</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D11">
         <v>1.25841E-3</v>
@@ -753,10 +804,14 @@
         <f t="shared" si="0"/>
         <v>1.3065899999999998E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>4595.9852236228153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D12">
         <v>1.3660199999999999E-3</v>
@@ -771,10 +826,14 @@
         <f t="shared" si="0"/>
         <v>1.3188133333333334E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <f>$G$2/G12</f>
+        <v>4553.38764141501</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D13">
         <v>1.07143E-3</v>
@@ -789,10 +848,14 @@
         <f t="shared" si="0"/>
         <v>1.1982366666666666E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>5011.5878610513792</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D14">
         <v>1.0226499999999999E-3</v>
@@ -804,13 +867,17 @@
         <v>1.24631E-3</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D14:F14)</f>
         <v>1.083161E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>5544.0219259494515</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D15">
         <v>1.32194E-3</v>
@@ -825,10 +892,14 @@
         <f t="shared" si="0"/>
         <v>1.2475833333333334E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>4813.3604969607914</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D16">
         <v>1.64496E-3</v>
@@ -843,10 +914,14 @@
         <f t="shared" si="0"/>
         <v>1.6000633333333335E-3</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>3753.0191513252603</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D17">
         <v>1.9673300000000002E-3</v>
@@ -861,13 +936,17 @@
         <f t="shared" si="0"/>
         <v>2.0120400000000001E-3</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>2984.5670728878817</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D18">
         <v>1.1684200000000001E-3</v>
@@ -882,13 +961,17 @@
         <f t="shared" si="0"/>
         <v>1.2683933333333334E-3</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>4734.3897003558313</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D19">
         <v>1.2450300000000001E-3</v>
@@ -903,13 +986,17 @@
         <f t="shared" si="0"/>
         <v>1.3627733333333332E-3</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>4406.5056062147787</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D20">
         <v>1.9991800000000001E-3</v>
@@ -924,13 +1011,17 @@
         <f t="shared" si="0"/>
         <v>2.2570233333333331E-3</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>2660.6142013005338</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D21">
         <v>1.3827900000000001E-3</v>
@@ -945,10 +1036,14 @@
         <f t="shared" si="0"/>
         <v>1.5268833333333335E-3</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>3932.8927117330509</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D22">
         <v>1.33373E-3</v>
@@ -963,18 +1058,22 @@
         <f t="shared" si="0"/>
         <v>1.3914333333333332E-3</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>4315.7427592650274</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C24" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="D23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="D24">
         <v>1.5023199999999999E-3</v>
@@ -989,10 +1088,14 @@
         <f t="shared" si="0"/>
         <v>1.4316399999999999E-3</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>4194.5379657828325</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D25">
         <v>1.4812899999999999E-3</v>
@@ -1007,10 +1110,14 @@
         <f t="shared" si="0"/>
         <v>1.5003833333333333E-3</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>4002.3560645612793</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C26" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D26">
         <v>1.61243E-3</v>
@@ -1025,10 +1132,14 @@
         <f t="shared" si="0"/>
         <v>1.5679733333333334E-3</v>
       </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>3829.8281008180411</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C27" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D27">
         <v>1.67282E-3</v>
@@ -1042,6 +1153,89 @@
       <c r="G27">
         <f t="shared" si="0"/>
         <v>1.4860033333333334E-3</v>
+      </c>
+      <c r="I27">
+        <f>$G$2/G27</f>
+        <v>4041.086718064787</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <f>AVERAGE(I3:I22,I24:I27)</f>
+        <v>3542.7531500763812</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>3</v>
+      </c>
+      <c r="G29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30">
+        <v>1.0226499999999999E-3</v>
+      </c>
+      <c r="E30">
+        <v>9.8052300000000007E-4</v>
+      </c>
+      <c r="F30">
+        <v>1.24631E-3</v>
+      </c>
+      <c r="G30">
+        <f>AVERAGE(D30:F30)</f>
+        <v>1.083161E-3</v>
+      </c>
+      <c r="I30">
+        <f>$G$2/G30</f>
+        <v>5544.0219259494515</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31">
+        <v>1.6097399999999999E-3</v>
+      </c>
+      <c r="E31">
+        <v>1.24807E-3</v>
+      </c>
+      <c r="F31">
+        <v>1.47708E-3</v>
+      </c>
+      <c r="G31">
+        <f>AVERAGE(D31:F31)</f>
+        <v>1.444963333333333E-3</v>
+      </c>
+      <c r="I31">
+        <f>$G$2/G31</f>
+        <v>4155.8620864658633</v>
       </c>
     </row>
   </sheetData>

</xml_diff>